<commit_message>
LOVE MY DEAR COUSIN. basic logics run through. LOVE MY DEAR COUSIN - MUST MARRY HIM AS SOON AS POSSIBLE
</commit_message>
<xml_diff>
--- a/Excel/StartSceneConfig@s.xlsx
+++ b/Excel/StartSceneConfig@s.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView windowWidth="28800" windowHeight="13500"/>
   </bookViews>
@@ -10,12 +10,12 @@
     <sheet name="StartSceneConfig" sheetId="1" r:id="rId1"/>
     <sheet name="Robot区" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr fullPrecision="1" calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24" count="52">
   <si>
     <t>Id</t>
   </si>
@@ -84,19 +84,22 @@
   </si>
   <si>
     <t>Robot01</t>
+  </si>
+  <si>
+    <t>Account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +128,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -201,7 +211,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
@@ -261,20 +271,231 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2B579A"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF2B579A"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="34">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
+  <fills count="35">
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E7E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -282,214 +503,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -504,15 +524,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,20 +545,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,223 +575,275 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF2B579A"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF2B579A"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyFont="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="5" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="9">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="51">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
+    <cellStyle name="Comma [0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27"/>
+    <cellStyle name="Comma" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - Accent3" xfId="9" builtinId="40"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="Percent" xfId="11" builtinId="5"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Note" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Warning Text" xfId="16" builtinId="11"/>
+    <cellStyle name="Title" xfId="17" builtinId="15"/>
+    <cellStyle name="Explanatory Text" xfId="18" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="19" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Heading 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - Accent4" xfId="23" builtinId="44"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="25" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - Accent6" xfId="27" builtinId="50"/>
+    <cellStyle name="Accent2" xfId="28" builtinId="33"/>
+    <cellStyle name="Linked Cell" xfId="29" builtinId="24"/>
+    <cellStyle name="Total" xfId="30" builtinId="25"/>
+    <cellStyle name="Good" xfId="31" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
+    <cellStyle name="Accent1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - Accent2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="38" builtinId="35"/>
+    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="ConditionalFormatStyle" xfId="49"/>
+    <cellStyle name="HeaderStyle" xfId="50"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
+  <tableStyles xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
@@ -1084,22 +1136,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="C3:H11"/>
+  <dimension ref="A3:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView view="normal" tabSelected="1" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="2" customWidth="1"/>
-    <col min="3" max="5" width="12.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.375" style="3" customWidth="1"/>
-    <col min="7" max="8" width="13.125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="21.16015625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.66015625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="12.66015625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="3" customWidth="1"/>
+    <col min="7" max="8" width="13.16015625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:8">
@@ -1162,7 +1214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="3:8">
+    <row r="6" spans="3:8" s="1" customFormat="1">
       <c r="C6" s="5">
         <v>1</v>
       </c>
@@ -1276,30 +1328,51 @@
       </c>
       <c r="H11" s="5"/>
     </row>
+    <row r="12" spans="3:8" ht="15">
+      <c r="C12" s="3">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="3">
+        <v>10005</v>
+      </c>
+    </row>
+    <row r="14" ht="15"/>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <headerFooter scaleWithDoc="1" alignWithMargins="1" differentFirst="0" differentOddEven="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="C3:H6"/>
+  <dimension ref="A3:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="$A6:$XFD6"/>
+    <sheetView view="normal" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="21.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="2" customWidth="1"/>
-    <col min="3" max="5" width="12.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.375" style="3" customWidth="1"/>
-    <col min="7" max="8" width="13.125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="21.16015625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.66015625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="12.66015625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="3" customWidth="1"/>
+    <col min="7" max="8" width="13.16015625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:8">
@@ -1362,7 +1435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="3:8">
+    <row r="6" spans="3:8" s="1" customFormat="1">
       <c r="C6" s="5">
         <v>200</v>
       </c>
@@ -1383,6 +1456,6 @@
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <headerFooter scaleWithDoc="1" alignWithMargins="1" differentFirst="0" differentOddEven="0"/>
 </worksheet>
 </file>
</xml_diff>